<commit_message>
ML Local Search / Hybrid PH-SDDP/ HeuristicYFixSDDP/SDDP
</commit_message>
<xml_diff>
--- a/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20_H010_c2.xlsx
+++ b/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20_H010_c2.xlsx
@@ -517,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -549,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1013</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>0.026</v>
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>181</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>0.026</v>
@@ -1690,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>301</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0.0248</v>
@@ -1725,7 +1725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1779,13 +1779,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>253</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1808,13 +1808,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>253</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1837,12 +1837,99 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
         <v>253</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H5" t="n">
         <v>45</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I5" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>253</v>
+      </c>
+      <c r="H6" t="n">
+        <v>45</v>
+      </c>
+      <c r="I6" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>253</v>
+      </c>
+      <c r="H7" t="n">
+        <v>45</v>
+      </c>
+      <c r="I7" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1857,7 +1944,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1911,13 +1998,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>36.62</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1940,13 +2027,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>36.62</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1969,12 +2056,99 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
         <v>36.62</v>
       </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>36.62</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>36.62</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>